<commit_message>
show tables and other interaction
</commit_message>
<xml_diff>
--- a/datasettings/loadpath/test.xlsx
+++ b/datasettings/loadpath/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\python\python_git\python-analysis\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\python\python_git\python-analysis\datasettings\loadpath\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1245,7 +1245,7 @@
         <v>423</v>
       </c>
       <c r="I2" s="1">
-        <v>43074.043761516201</v>
+        <v>42767</v>
       </c>
       <c r="J2" t="s">
         <v>43</v>
@@ -1277,7 +1277,7 @@
         <v>1234</v>
       </c>
       <c r="I3" s="1">
-        <v>43075.043761516201</v>
+        <v>42768</v>
       </c>
       <c r="J3" t="s">
         <v>44</v>
@@ -1309,7 +1309,7 @@
         <v>1234</v>
       </c>
       <c r="I4" s="1">
-        <v>43076.043761516201</v>
+        <v>42769</v>
       </c>
       <c r="J4" t="s">
         <v>45</v>
@@ -1341,7 +1341,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="1">
-        <v>43077.043761516201</v>
+        <v>42770</v>
       </c>
       <c r="J5" t="s">
         <v>46</v>
@@ -1373,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="I6" s="1">
-        <v>43078.043761516201</v>
+        <v>42773</v>
       </c>
       <c r="J6" t="s">
         <v>53</v>
@@ -1405,7 +1405,7 @@
         <v>21</v>
       </c>
       <c r="I7" s="1">
-        <v>43079.043761516201</v>
+        <v>42774</v>
       </c>
       <c r="J7" t="s">
         <v>47</v>
@@ -1434,7 +1434,7 @@
         <v>134</v>
       </c>
       <c r="I8" s="1">
-        <v>43080.043761516201</v>
+        <v>42775</v>
       </c>
       <c r="J8" t="s">
         <v>54</v>
@@ -1460,7 +1460,7 @@
         <v>5364</v>
       </c>
       <c r="I9" s="1">
-        <v>43081.043761458335</v>
+        <v>42783</v>
       </c>
       <c r="J9" t="s">
         <v>48</v>
@@ -1492,7 +1492,7 @@
         <v>42</v>
       </c>
       <c r="I10" s="1">
-        <v>43082.043761458335</v>
+        <v>42784</v>
       </c>
       <c r="J10" t="s">
         <v>49</v>
@@ -1524,7 +1524,7 @@
         <v>43</v>
       </c>
       <c r="I11" s="1">
-        <v>43076.043761516201</v>
+        <v>42785</v>
       </c>
       <c r="J11" t="s">
         <v>52</v>
@@ -1550,7 +1550,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="1">
-        <v>43077.043761516201</v>
+        <v>42786</v>
       </c>
       <c r="J12" t="s">
         <v>50</v>
@@ -1576,7 +1576,7 @@
         <v>43081.043761458335</v>
       </c>
       <c r="I13" s="1">
-        <v>43078.043761516201</v>
+        <v>42787</v>
       </c>
       <c r="J13" t="s">
         <v>55</v>
@@ -1608,7 +1608,7 @@
         <v>36</v>
       </c>
       <c r="I14" s="1">
-        <v>43079.043761516201</v>
+        <v>42790</v>
       </c>
       <c r="J14" t="s">
         <v>59</v>
@@ -1637,7 +1637,7 @@
         <v>134</v>
       </c>
       <c r="I15" s="1">
-        <v>43080.043761516201</v>
+        <v>42791</v>
       </c>
       <c r="J15" t="s">
         <v>51</v>
@@ -1669,7 +1669,7 @@
         <v>5364</v>
       </c>
       <c r="I16" s="1">
-        <v>43074.043761516201</v>
+        <v>42792</v>
       </c>
       <c r="J16" t="s">
         <v>56</v>
@@ -1701,7 +1701,7 @@
         <v>42</v>
       </c>
       <c r="I17" s="1">
-        <v>43075.043761516201</v>
+        <v>42795</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
@@ -1730,7 +1730,7 @@
         <v>43</v>
       </c>
       <c r="I18" s="1">
-        <v>43076.043761516201</v>
+        <v>42796</v>
       </c>
       <c r="J18" t="s">
         <v>57</v>
@@ -1759,7 +1759,7 @@
         <v>25</v>
       </c>
       <c r="I19" s="1">
-        <v>43077.043761516201</v>
+        <v>42797</v>
       </c>
       <c r="J19" t="s">
         <v>58</v>
@@ -1785,7 +1785,7 @@
         <v>43088.043761458335</v>
       </c>
       <c r="I20" s="1">
-        <v>43078.043761516201</v>
+        <v>42798</v>
       </c>
       <c r="J20">
         <v>4</v>

</xml_diff>